<commit_message>
Fixed typo in Byrnes 2014 NE Appledore Swath and fish mis-identifying a transect as being in NW Appledore
</commit_message>
<xml_diff>
--- a/raw_data/KEEN ONE/Byrnes/2014/NE Shoals Entry 2014/NE Shoals Swath.xlsx
+++ b/raw_data/KEEN ONE/Byrnes/2014/NE Shoals Entry 2014/NE Shoals Swath.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="133">
   <si>
     <t>un-readable*</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -246,10 +246,6 @@
   </si>
   <si>
     <t>HESA</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>NW Appledore</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
@@ -893,7 +889,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -983,6 +979,18 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1012,11 +1020,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1092,9 +1102,11 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1496,8 +1508,8 @@
   <dimension ref="A1:T10046"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="N1" sqref="N1:N1048576"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1520,61 +1532,61 @@
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -1591,13 +1603,13 @@
         <v>41839</v>
       </c>
       <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
         <v>36</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>37</v>
-      </c>
-      <c r="G2" t="s">
-        <v>38</v>
       </c>
       <c r="H2"/>
       <c r="I2"/>
@@ -1608,10 +1620,10 @@
         <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P2">
         <v>10.8</v>
@@ -1643,13 +1655,13 @@
         <v>41839</v>
       </c>
       <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
         <v>36</v>
       </c>
-      <c r="F3" t="s">
-        <v>37</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -1660,10 +1672,10 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P3">
         <v>10.8</v>
@@ -1692,13 +1704,13 @@
         <v>41839</v>
       </c>
       <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
         <v>36</v>
       </c>
-      <c r="F4" t="s">
-        <v>37</v>
-      </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -1713,10 +1725,10 @@
         <v>4</v>
       </c>
       <c r="L4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P4">
         <v>10.8</v>
@@ -1745,13 +1757,13 @@
         <v>41839</v>
       </c>
       <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5"/>
       <c r="I5">
@@ -1764,10 +1776,10 @@
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P5">
         <v>10.8</v>
@@ -1796,13 +1808,13 @@
         <v>41839</v>
       </c>
       <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
         <v>36</v>
       </c>
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -1812,10 +1824,10 @@
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P6">
         <v>10.8</v>
@@ -1844,13 +1856,13 @@
         <v>41839</v>
       </c>
       <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
         <v>36</v>
       </c>
-      <c r="F7" t="s">
-        <v>37</v>
-      </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H7"/>
       <c r="I7"/>
@@ -1858,10 +1870,10 @@
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P7">
         <v>10.8</v>
@@ -1890,13 +1902,13 @@
         <v>41839</v>
       </c>
       <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
         <v>36</v>
       </c>
-      <c r="F8" t="s">
-        <v>37</v>
-      </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8"/>
       <c r="I8">
@@ -1906,10 +1918,10 @@
         <v>11</v>
       </c>
       <c r="L8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P8">
         <v>10.8</v>
@@ -1938,13 +1950,13 @@
         <v>41839</v>
       </c>
       <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
         <v>36</v>
       </c>
-      <c r="F9" t="s">
-        <v>37</v>
-      </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1959,10 +1971,10 @@
         <v>5</v>
       </c>
       <c r="L9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P9">
         <v>10.8</v>
@@ -1997,13 +2009,13 @@
         <v>41838</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11">
         <v>3</v>
@@ -2012,10 +2024,10 @@
         <v>2</v>
       </c>
       <c r="L11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P11">
         <v>6</v>
@@ -2047,23 +2059,23 @@
         <v>41838</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="I12"/>
       <c r="L12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P12">
         <v>6</v>
@@ -2092,13 +2104,13 @@
         <v>41838</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H13">
         <v>7</v>
@@ -2107,10 +2119,10 @@
         <v>7</v>
       </c>
       <c r="L13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P13">
         <v>6</v>
@@ -2139,23 +2151,23 @@
         <v>41838</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" t="s">
         <v>49</v>
-      </c>
-      <c r="G14" t="s">
-        <v>50</v>
       </c>
       <c r="H14">
         <v>2</v>
       </c>
       <c r="I14"/>
       <c r="L14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P14">
         <v>6</v>
@@ -2184,23 +2196,23 @@
         <v>41838</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="I15"/>
       <c r="L15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P15">
         <v>6</v>
@@ -2229,23 +2241,23 @@
         <v>41838</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H16">
         <v>2</v>
       </c>
       <c r="I16"/>
       <c r="L16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P16">
         <v>6</v>
@@ -2274,13 +2286,13 @@
         <v>41838</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J17">
         <v>4</v>
@@ -2289,10 +2301,10 @@
         <v>1</v>
       </c>
       <c r="L17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P17">
         <v>25</v>
@@ -2324,22 +2336,22 @@
         <v>41838</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J18">
         <v>1</v>
       </c>
       <c r="L18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P18">
         <v>25</v>
@@ -2368,13 +2380,13 @@
         <v>41838</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J19">
         <v>12</v>
@@ -2383,10 +2395,10 @@
         <v>4</v>
       </c>
       <c r="L19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P19">
         <v>25</v>
@@ -2415,22 +2427,22 @@
         <v>41838</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K20">
         <v>1</v>
       </c>
       <c r="L20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P20">
         <v>25</v>
@@ -2466,13 +2478,13 @@
         <v>41841</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" t="s">
         <v>6</v>
       </c>
       <c r="G22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H22" s="6">
         <v>2</v>
@@ -2481,10 +2493,10 @@
         <v>11</v>
       </c>
       <c r="L22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P22">
         <v>11.4</v>
@@ -2516,22 +2528,22 @@
         <v>41841</v>
       </c>
       <c r="E23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F23" t="s">
         <v>6</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I23" s="6">
         <v>2</v>
       </c>
       <c r="L23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P23">
         <v>11.4</v>
@@ -2560,13 +2572,13 @@
         <v>41841</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F24" t="s">
         <v>6</v>
       </c>
       <c r="G24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H24" s="6">
         <v>2</v>
@@ -2575,10 +2587,10 @@
         <v>3</v>
       </c>
       <c r="L24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P24">
         <v>11.4</v>
@@ -2607,7 +2619,7 @@
         <v>41841</v>
       </c>
       <c r="E25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F25" t="s">
         <v>6</v>
@@ -2622,10 +2634,10 @@
         <v>1</v>
       </c>
       <c r="L25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P25">
         <v>11.4</v>
@@ -2654,13 +2666,13 @@
         <v>41841</v>
       </c>
       <c r="E26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F26" t="s">
         <v>6</v>
       </c>
       <c r="G26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H26" s="6">
         <v>2</v>
@@ -2669,10 +2681,10 @@
         <v>2</v>
       </c>
       <c r="L26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P26">
         <v>11.4</v>
@@ -2701,7 +2713,7 @@
         <v>41841</v>
       </c>
       <c r="E27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F27" t="s">
         <v>6</v>
@@ -2716,10 +2728,10 @@
         <v>1</v>
       </c>
       <c r="L27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P27">
         <v>11.4</v>
@@ -2748,13 +2760,13 @@
         <v>41841</v>
       </c>
       <c r="E28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F28" t="s">
         <v>6</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H28" s="6">
         <v>11</v>
@@ -2763,10 +2775,10 @@
         <v>53</v>
       </c>
       <c r="L28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P28">
         <v>11.4</v>
@@ -2795,13 +2807,13 @@
         <v>41841</v>
       </c>
       <c r="E29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F29" t="s">
         <v>6</v>
       </c>
       <c r="G29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J29">
         <v>5</v>
@@ -2813,7 +2825,7 @@
         <v>9</v>
       </c>
       <c r="N29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P29">
         <v>11.4</v>
@@ -2842,13 +2854,13 @@
         <v>41841</v>
       </c>
       <c r="E30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F30" t="s">
         <v>6</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -2857,7 +2869,7 @@
         <v>9</v>
       </c>
       <c r="N30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P30">
         <v>11.4</v>
@@ -2886,13 +2898,13 @@
         <v>41841</v>
       </c>
       <c r="E31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F31" t="s">
         <v>6</v>
       </c>
       <c r="G31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J31">
         <v>3</v>
@@ -2904,7 +2916,7 @@
         <v>9</v>
       </c>
       <c r="N31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P31">
         <v>11.4</v>
@@ -2933,7 +2945,7 @@
         <v>41841</v>
       </c>
       <c r="E32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F32" t="s">
         <v>6</v>
@@ -2951,7 +2963,7 @@
         <v>9</v>
       </c>
       <c r="N32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P32">
         <v>11.4</v>
@@ -2980,19 +2992,19 @@
         <v>41841</v>
       </c>
       <c r="E33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F33" t="s">
         <v>6</v>
       </c>
       <c r="G33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L33" t="s">
         <v>9</v>
       </c>
       <c r="N33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P33">
         <v>11.4</v>
@@ -3021,7 +3033,7 @@
         <v>41841</v>
       </c>
       <c r="E34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F34" t="s">
         <v>6</v>
@@ -3039,7 +3051,7 @@
         <v>9</v>
       </c>
       <c r="N34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P34">
         <v>11.4</v>
@@ -3068,7 +3080,7 @@
         <v>41841</v>
       </c>
       <c r="E35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F35" t="s">
         <v>6</v>
@@ -3083,7 +3095,7 @@
         <v>9</v>
       </c>
       <c r="N35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P35">
         <v>11.4</v>
@@ -3119,13 +3131,13 @@
         <v>41838</v>
       </c>
       <c r="E37" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" t="s">
         <v>12</v>
       </c>
-      <c r="F37" t="s">
-        <v>13</v>
-      </c>
       <c r="G37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H37" s="6">
         <v>1</v>
@@ -3134,13 +3146,13 @@
         <v>1</v>
       </c>
       <c r="L37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P37">
         <v>30</v>
@@ -3172,22 +3184,22 @@
         <v>41838</v>
       </c>
       <c r="E38" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" t="s">
         <v>12</v>
       </c>
-      <c r="F38" t="s">
-        <v>13</v>
-      </c>
       <c r="G38" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P38">
         <v>30</v>
@@ -3216,13 +3228,13 @@
         <v>41838</v>
       </c>
       <c r="E39" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" t="s">
         <v>12</v>
       </c>
-      <c r="F39" t="s">
-        <v>13</v>
-      </c>
       <c r="G39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H39" s="6">
         <v>3</v>
@@ -3231,10 +3243,10 @@
         <v>6</v>
       </c>
       <c r="L39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P39">
         <v>30</v>
@@ -3263,25 +3275,25 @@
         <v>41838</v>
       </c>
       <c r="E40" t="s">
+        <v>35</v>
+      </c>
+      <c r="F40" t="s">
         <v>12</v>
       </c>
-      <c r="F40" t="s">
-        <v>13</v>
-      </c>
       <c r="G40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H40" s="6">
         <v>1</v>
       </c>
       <c r="L40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M40" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P40">
         <v>30</v>
@@ -3310,13 +3322,13 @@
         <v>41838</v>
       </c>
       <c r="E41" t="s">
+        <v>35</v>
+      </c>
+      <c r="F41" t="s">
         <v>12</v>
       </c>
-      <c r="F41" t="s">
-        <v>13</v>
-      </c>
       <c r="G41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H41" s="6">
         <v>1</v>
@@ -3325,10 +3337,10 @@
         <v>8</v>
       </c>
       <c r="L41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P41">
         <v>30</v>
@@ -3357,22 +3369,22 @@
         <v>41838</v>
       </c>
       <c r="E42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F42" t="s">
         <v>12</v>
       </c>
-      <c r="F42" t="s">
-        <v>13</v>
-      </c>
       <c r="G42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H42" s="6">
         <v>2</v>
       </c>
       <c r="L42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P42">
         <v>30</v>
@@ -3401,10 +3413,10 @@
         <v>41838</v>
       </c>
       <c r="E43" t="s">
+        <v>35</v>
+      </c>
+      <c r="F43" t="s">
         <v>12</v>
-      </c>
-      <c r="F43" t="s">
-        <v>13</v>
       </c>
       <c r="G43" s="33" t="s">
         <v>0</v>
@@ -3413,10 +3425,10 @@
         <v>1</v>
       </c>
       <c r="L43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P43">
         <v>30</v>
@@ -3445,22 +3457,22 @@
         <v>41838</v>
       </c>
       <c r="E44" t="s">
+        <v>35</v>
+      </c>
+      <c r="F44" t="s">
         <v>12</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>13</v>
-      </c>
-      <c r="G44" t="s">
-        <v>14</v>
       </c>
       <c r="I44" s="6">
         <v>2</v>
       </c>
       <c r="L44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P44">
         <v>30</v>
@@ -3489,22 +3501,22 @@
         <v>41838</v>
       </c>
       <c r="E45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F45" t="s">
         <v>12</v>
       </c>
-      <c r="F45" t="s">
-        <v>13</v>
-      </c>
       <c r="G45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I45" s="6">
         <v>1</v>
       </c>
       <c r="L45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P45">
         <v>30</v>
@@ -3533,19 +3545,19 @@
         <v>41838</v>
       </c>
       <c r="E46" t="s">
+        <v>35</v>
+      </c>
+      <c r="F46" t="s">
         <v>12</v>
       </c>
-      <c r="F46" t="s">
-        <v>13</v>
-      </c>
       <c r="G46" t="s">
+        <v>37</v>
+      </c>
+      <c r="L46" t="s">
+        <v>41</v>
+      </c>
+      <c r="N46" t="s">
         <v>38</v>
-      </c>
-      <c r="L46" t="s">
-        <v>42</v>
-      </c>
-      <c r="N46" t="s">
-        <v>39</v>
       </c>
       <c r="P46">
         <v>9.8000000000000007</v>
@@ -3574,19 +3586,19 @@
         <v>41838</v>
       </c>
       <c r="E47" t="s">
+        <v>35</v>
+      </c>
+      <c r="F47" t="s">
         <v>12</v>
       </c>
-      <c r="F47" t="s">
-        <v>13</v>
-      </c>
       <c r="G47" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L47" t="s">
         <v>41</v>
       </c>
-      <c r="L47" t="s">
-        <v>42</v>
-      </c>
       <c r="N47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P47">
         <v>9.8000000000000007</v>
@@ -3615,22 +3627,22 @@
         <v>41838</v>
       </c>
       <c r="E48" t="s">
+        <v>35</v>
+      </c>
+      <c r="F48" t="s">
         <v>12</v>
       </c>
-      <c r="F48" t="s">
-        <v>13</v>
-      </c>
       <c r="G48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J48">
         <v>2</v>
       </c>
       <c r="L48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P48">
         <v>9.8000000000000007</v>
@@ -3659,10 +3671,10 @@
         <v>41838</v>
       </c>
       <c r="E49" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49" t="s">
         <v>12</v>
-      </c>
-      <c r="F49" t="s">
-        <v>13</v>
       </c>
       <c r="G49" t="s">
         <v>7</v>
@@ -3671,10 +3683,10 @@
         <v>2</v>
       </c>
       <c r="L49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N49" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P49">
         <v>9.8000000000000007</v>
@@ -3703,19 +3715,19 @@
         <v>41838</v>
       </c>
       <c r="E50" t="s">
+        <v>35</v>
+      </c>
+      <c r="F50" t="s">
         <v>12</v>
       </c>
-      <c r="F50" t="s">
-        <v>13</v>
-      </c>
       <c r="G50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N50" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P50">
         <v>9.8000000000000007</v>
@@ -3744,19 +3756,19 @@
         <v>41838</v>
       </c>
       <c r="E51" t="s">
+        <v>35</v>
+      </c>
+      <c r="F51" t="s">
         <v>12</v>
       </c>
-      <c r="F51" t="s">
-        <v>13</v>
-      </c>
       <c r="G51" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L51" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N51" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P51">
         <v>9.8000000000000007</v>
@@ -3785,13 +3797,13 @@
         <v>41838</v>
       </c>
       <c r="E52" t="s">
+        <v>35</v>
+      </c>
+      <c r="F52" t="s">
         <v>12</v>
       </c>
-      <c r="F52" t="s">
-        <v>13</v>
-      </c>
       <c r="G52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J52">
         <v>6</v>
@@ -3800,10 +3812,10 @@
         <v>5</v>
       </c>
       <c r="L52" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P52">
         <v>9.8000000000000007</v>
@@ -3832,22 +3844,22 @@
         <v>41838</v>
       </c>
       <c r="E53" t="s">
+        <v>35</v>
+      </c>
+      <c r="F53" t="s">
         <v>12</v>
       </c>
-      <c r="F53" t="s">
-        <v>13</v>
-      </c>
       <c r="G53" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K53">
         <v>2</v>
       </c>
       <c r="L53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P53">
         <v>9.8000000000000007</v>
@@ -4099,94 +4111,94 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="14"/>
       <c r="B2" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C3" s="16"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>82</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>83</v>
       </c>
       <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="18"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="18"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="18"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="18"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="18"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>5</v>
@@ -4196,56 +4208,56 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="18"/>
       <c r="B14" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="18"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
@@ -4254,10 +4266,10 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
@@ -4268,7 +4280,7 @@
     <row r="19" spans="1:11">
       <c r="A19" s="23"/>
       <c r="B19" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="18"/>
@@ -4281,139 +4293,139 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" s="24"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="24"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="18"/>
       <c r="B27" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C27" s="18"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="C28" s="13" t="s">
         <v>103</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>104</v>
       </c>
       <c r="D28" s="25"/>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="C29" s="13" t="s">
         <v>107</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>108</v>
       </c>
       <c r="D29" s="18"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="C30" s="13" t="s">
         <v>111</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>112</v>
       </c>
       <c r="D30" s="18"/>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="C31" s="13" t="s">
         <v>115</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>116</v>
       </c>
       <c r="D31" s="29"/>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="C32" s="13" t="s">
         <v>119</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>120</v>
       </c>
       <c r="D32" s="18"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" s="16" t="s">
         <v>122</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>123</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
@@ -4427,58 +4439,58 @@
     <row r="36" spans="1:4">
       <c r="A36" s="23"/>
       <c r="B36" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" s="18"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="16" t="s">
         <v>80</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>81</v>
       </c>
       <c r="C37" s="18"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C38" s="18"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:4">

</xml_diff>